<commit_message>
ndimas add signup test page
</commit_message>
<xml_diff>
--- a/assets/data/account.xlsx
+++ b/assets/data/account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew\flutter_application_1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ACF38C-FAF5-45F4-9ECB-DC081B3261AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8BBF12-6B10-4660-9FD8-8C19654B541A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="276" windowWidth="16332" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,7 +415,7 @@
     <col min="5" max="5" width="13.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +431,11 @@
       <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -448,8 +451,11 @@
       <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -465,8 +471,11 @@
       <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -481,6 +490,9 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="F4">
+        <v>17000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ndimas add date fix bug
</commit_message>
<xml_diff>
--- a/assets/data/account.xlsx
+++ b/assets/data/account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew\flutter_application_1\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riand\Documents\tmp\flutter_app\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8BBF12-6B10-4660-9FD8-8C19654B541A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4FAC54-8DC7-4546-97AB-1F265445418F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="276" windowWidth="16332" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Ndimas</t>
   </si>
@@ -82,16 +82,34 @@
   </si>
   <si>
     <t>081375722604</t>
+  </si>
+  <si>
+    <t>1/1/2000</t>
+  </si>
+  <si>
+    <t>12/12/2000</t>
+  </si>
+  <si>
+    <t>15/3/2000</t>
+  </si>
+  <si>
+    <t>12/1/2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,10 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,21 +421,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.90625" style="1"/>
+    <col min="3" max="3" width="31.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +455,11 @@
       <c r="F1">
         <v>0</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -454,8 +478,11 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -474,8 +501,11 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -494,8 +524,12 @@
       <c r="F4">
         <v>17000</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>